<commit_message>
update fits and data
</commit_message>
<xml_diff>
--- a/National_Measles_Cases_Weekly_2025.xlsx
+++ b/National_Measles_Cases_Weekly_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/263e6c96784ab765/Desktop/Common_Health/Measles_USA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{AC3AAFDE-5832-4E94-8956-120FA1D4CDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0E06048-4E91-40AF-A396-A89E4FEF386B}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{AC3AAFDE-5832-4E94-8956-120FA1D4CDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAEB7DA3-92A2-433B-95FC-D5A494022031}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F85433EA-CC4E-448A-82CB-0B2B9491D978}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F85433EA-CC4E-448A-82CB-0B2B9491D978}"/>
   </bookViews>
   <sheets>
     <sheet name="National_Measles_Cases_Weekly" sheetId="1" r:id="rId1"/>
@@ -597,6 +597,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -918,7 +922,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8AAB0C-CA42-4832-8EA4-1AB4201B529F}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1477,8 +1483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{186E4C24-AA43-497C-B947-791C0C13EFB7}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update data and optimization function
</commit_message>
<xml_diff>
--- a/National_Measles_Cases_Weekly_2025.xlsx
+++ b/National_Measles_Cases_Weekly_2025.xlsx
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/263e6c96784ab765/Desktop/Common_Health/Measles_USA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{AC3AAFDE-5832-4E94-8956-120FA1D4CDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAEB7DA3-92A2-433B-95FC-D5A494022031}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{AC3AAFDE-5832-4E94-8956-120FA1D4CDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71AAF8F6-8108-4A98-8199-1FE93883C169}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F85433EA-CC4E-448A-82CB-0B2B9491D978}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F85433EA-CC4E-448A-82CB-0B2B9491D978}"/>
   </bookViews>
   <sheets>
     <sheet name="National_Measles_Cases_Weekly" sheetId="1" r:id="rId1"/>
     <sheet name="Sources" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>EpiWeek</t>
   </si>
@@ -29,19 +42,7 @@
     <t>total_cases</t>
   </si>
   <si>
-    <t>imported_cases</t>
-  </si>
-  <si>
-    <t>local_cases</t>
-  </si>
-  <si>
     <t>https://publichealth.jhu.edu/ivac/resources/us-measles-tracker</t>
-  </si>
-  <si>
-    <t>https://data.cdc.gov/NNDSS/NNDSS-Weekly-Data/x9gk-5huc/data_preview</t>
-  </si>
-  <si>
-    <t>Imported</t>
   </si>
   <si>
     <t>Total</t>
@@ -920,558 +921,356 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8AAB0C-CA42-4832-8EA4-1AB4201B529F}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>12</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>23</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>28</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>65</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>76</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>76</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>79</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>93</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>102</v>
       </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>91</v>
       </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>107</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>91</v>
       </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>66</v>
       </c>
-      <c r="C16">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>48</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>47</v>
       </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="D18">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
         <v>47</v>
       </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
         <v>23</v>
       </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <v>40</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
         <v>35</v>
       </c>
-      <c r="C22">
-        <v>5</v>
-      </c>
-      <c r="D22">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
         <v>34</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
         <v>25</v>
       </c>
-      <c r="C24">
-        <v>8</v>
-      </c>
-      <c r="D24">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
-      <c r="C25">
-        <v>13</v>
-      </c>
-      <c r="D25">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
         <v>37</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
         <v>25</v>
       </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
         <v>13</v>
       </c>
-      <c r="C28">
-        <v>6</v>
-      </c>
-      <c r="D28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
         <v>9</v>
       </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-      <c r="D29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
         <v>16</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
         <v>17</v>
       </c>
-      <c r="C31">
-        <v>6</v>
-      </c>
-      <c r="D31">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
         <v>6</v>
       </c>
-      <c r="C32">
-        <v>4</v>
-      </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
         <v>15</v>
       </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
         <v>37</v>
       </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
         <v>20</v>
       </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
         <v>20</v>
       </c>
-      <c r="C36">
-        <v>13</v>
-      </c>
-      <c r="D36">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
         <v>32</v>
       </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
         <v>24</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
         <v>23</v>
       </c>
-      <c r="C39">
-        <v>3</v>
-      </c>
-      <c r="D39">
-        <v>20</v>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1483,7 +1282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{186E4C24-AA43-497C-B947-791C0C13EFB7}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -1491,24 +1290,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{06DFC55F-6123-47AB-A37A-6713370A2BE9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>